<commit_message>
Update of numbers in paper
</commit_message>
<xml_diff>
--- a/Tables/exp_arms.xlsx
+++ b/Tables/exp_arms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\SEIRA\donde2019\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xps-seira\Dropbox\Apps\ShareLaTeX\Donde2019\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB9CCB0-7871-40AA-9D28-630AA6FF4482}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62343C5F-41D1-439F-80B0-ABE167D78815}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{47361F37-7346-447C-B942-BB91466DC8E5}"/>
+    <workbookView xWindow="-13872" yWindow="-13068" windowWidth="23256" windowHeight="13176" xr2:uid="{47361F37-7346-447C-B942-BB91466DC8E5}"/>
   </bookViews>
   <sheets>
     <sheet name="exp_arms" sheetId="1" r:id="rId1"/>
@@ -273,18 +273,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -294,25 +309,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -618,11 +618,72 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>300037</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>18950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>271463</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>51436</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1941BC29-D561-473B-91EA-9FBBA382265F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2171700" y="1533425"/>
+          <a:ext cx="4338638" cy="1842236"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -920,93 +981,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A5DD533-5204-420F-8403-FC827585B082}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="160" zoomScaleNormal="190" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="160" zoomScaleNormal="190" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="16"/>
+      <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="17">
         <v>2484</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="12">
-        <v>3089</v>
+      <c r="C2" s="18"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="6">
+        <v>3088</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="18">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="15"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="8">
         <v>347</v>
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="13">
-        <v>2156</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="17"/>
+      <c r="B4" s="17">
+        <v>2157</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="3">
-        <v>1909</v>
+        <v>1908</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="18">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="8">
         <v>859</v>
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="9">
         <v>2601</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>

</xml_diff>